<commit_message>
perubahan data impor pada catatan keluarga
</commit_message>
<xml_diff>
--- a/assets_dasa_wisma/contoh.xlsx
+++ b/assets_dasa_wisma/contoh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Kominfo-DS\Website\dasa-wisma\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\WebsiteDesa\assets_dasa_wisma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2CAA03-C58E-40A0-A1C0-B9EEBD311434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D438D596-943A-4AB2-B087-1FDF84DD8742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CF6C1600-5A86-4ED3-B8E1-631C36680964}"/>
   </bookViews>
@@ -393,52 +393,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81454CA2-FD6A-49AA-9E69-4DD390FEE9E7}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
+    <col min="1" max="13" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="2">
         <v>112233445566</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2">
+        <v>3</v>
+      </c>
+      <c r="K1" s="2">
+        <v>1</v>
+      </c>
+      <c r="L1" s="2">
+        <v>2</v>
+      </c>
+      <c r="M1" s="2">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2">
+      <c r="O1" s="2">
+        <v>2</v>
+      </c>
+      <c r="P1" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="2">
+      <c r="T1" s="2">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1">
+      <c r="U1" t="s">
+        <v>2</v>
+      </c>
+      <c r="V1" s="1">
         <v>44963</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J12" t="s">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="V12" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>